<commit_message>
Ajustes casa 04-04-2025 2000
</commit_message>
<xml_diff>
--- a/public/files/Todos los Componentes Reg. Oriental.xlsx
+++ b/public/files/Todos los Componentes Reg. Oriental.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATOS120GBW10\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto\sisoe\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ECCC4D-73A9-4A92-A815-063C16693641}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F878B8E-C4F4-4F2A-AF10-18E2A73832D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="339">
   <si>
     <t>component_id</t>
   </si>
@@ -2221,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="A508" sqref="A508"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3120,8 +3120,8 @@
       <c r="B20" s="7">
         <v>9999</v>
       </c>
-      <c r="C20" s="7">
-        <v>1</v>
+      <c r="C20" s="12">
+        <v>19</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
@@ -3167,7 +3167,7 @@
         <v>9999</v>
       </c>
       <c r="C21" s="12">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D21" s="13">
         <v>2</v>
@@ -3213,7 +3213,7 @@
         <v>9999</v>
       </c>
       <c r="C22" s="12">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D22" s="13">
         <v>3</v>
@@ -3259,7 +3259,7 @@
         <v>9999</v>
       </c>
       <c r="C23" s="12">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D23" s="13">
         <v>4</v>
@@ -3305,7 +3305,7 @@
         <v>9999</v>
       </c>
       <c r="C24" s="12">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D24" s="13">
         <v>5</v>
@@ -3351,7 +3351,7 @@
         <v>9999</v>
       </c>
       <c r="C25" s="12">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D25" s="13">
         <v>6</v>
@@ -3397,7 +3397,7 @@
         <v>9999</v>
       </c>
       <c r="C26" s="12">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D26" s="13">
         <v>7</v>
@@ -3443,7 +3443,7 @@
         <v>9999</v>
       </c>
       <c r="C27" s="12">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D27" s="13">
         <v>8</v>
@@ -3489,7 +3489,7 @@
         <v>9999</v>
       </c>
       <c r="C28" s="12">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D28" s="13">
         <v>9</v>
@@ -3535,7 +3535,7 @@
         <v>9999</v>
       </c>
       <c r="C29" s="12">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D29" s="13">
         <v>10</v>
@@ -3581,7 +3581,7 @@
         <v>9999</v>
       </c>
       <c r="C30" s="12">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D30" s="13">
         <v>11</v>
@@ -3627,7 +3627,7 @@
         <v>9999</v>
       </c>
       <c r="C31" s="12">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D31" s="13">
         <v>12</v>
@@ -3673,7 +3673,7 @@
         <v>9999</v>
       </c>
       <c r="C32" s="12">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D32" s="13">
         <v>13</v>
@@ -3719,7 +3719,7 @@
         <v>9999</v>
       </c>
       <c r="C33" s="12">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D33" s="13">
         <v>14</v>
@@ -3765,7 +3765,7 @@
         <v>9999</v>
       </c>
       <c r="C34" s="12">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D34" s="13">
         <v>15</v>

</xml_diff>